<commit_message>
updated for spring 2024
</commit_message>
<xml_diff>
--- a/Research-Project/final-rubric.xlsx
+++ b/Research-Project/final-rubric.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/dbhagia/Dropbox (CSU Fullerton)/Teaching/Econ340/Research-Project/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D487979B-73C2-BA4B-B7A7-440EE1D34420}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A4447CF6-76FE-414E-B73D-7A1CD5F6F6F4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="5180" yWindow="500" windowWidth="30080" windowHeight="19960" xr2:uid="{5F5E5395-EDEE-AA41-90EB-5510CF5BE07E}"/>
+    <workbookView xWindow="38400" yWindow="500" windowWidth="38400" windowHeight="21100" xr2:uid="{5F5E5395-EDEE-AA41-90EB-5510CF5BE07E}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -815,8 +815,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{170BC48A-5C7A-1941-956A-C10534CD8C16}">
   <dimension ref="A1:E25"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="119" zoomScaleNormal="119" workbookViewId="0">
-      <selection activeCell="B6" sqref="B6"/>
+    <sheetView tabSelected="1" topLeftCell="A15" zoomScale="166" zoomScaleNormal="166" workbookViewId="0">
+      <selection activeCell="B19" sqref="B19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="60" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -1080,7 +1080,7 @@
         <v>47</v>
       </c>
     </row>
-    <row r="17" spans="1:5" ht="60" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:5" ht="81" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A17" s="6"/>
       <c r="B17" s="3" t="s">
         <v>85</v>

</xml_diff>

<commit_message>
added rubric for final submission and some other minor edits
</commit_message>
<xml_diff>
--- a/Research-Project/final-rubric.xlsx
+++ b/Research-Project/final-rubric.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10414"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11027"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/dbhagia/Dropbox (CSU Fullerton)/Teaching/Econ340/Research-Project/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/dbhagia/CSU Fullerton Dropbox/Div Bhagia/Teaching/Econ340/Research-Project/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{28BF80CE-37E6-224F-9472-991A7ABD8845}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6FA75D9A-EF3A-774B-AD77-61905F5CBD47}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="500" windowWidth="38400" windowHeight="19480" xr2:uid="{5F5E5395-EDEE-AA41-90EB-5510CF5BE07E}"/>
   </bookViews>
@@ -815,8 +815,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{170BC48A-5C7A-1941-956A-C10534CD8C16}">
   <dimension ref="A1:E25"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A17" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <selection activeCell="B18" sqref="B18"/>
+    <sheetView tabSelected="1" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
+      <selection activeCell="B4" sqref="B4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="60" customHeight="1" x14ac:dyDescent="0.2"/>

</xml_diff>